<commit_message>
updated for non dig env
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pauldawson/Desktop/development/funky-spreadsheet-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{198158E3-013B-E847-A737-9A671F2701ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1994B8AD-3A5A-9640-9E17-89B3EEB743EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{BF88B243-FB9B-1246-8726-7BC6AB377249}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="93">
   <si>
     <t>CC_1_RAWTOHEX__UUID__</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>d3bxschxt4niqn.cloudfront.net</t>
+  </si>
+  <si>
+    <t>google.com</t>
   </si>
 </sst>
 </file>
@@ -694,13 +697,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CE3B63-7973-254B-A7D9-2657A67FFD7D}">
-  <dimension ref="A1:BJ4"/>
+  <dimension ref="A1:BJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1409,6 +1415,179 @@
         <v>1</v>
       </c>
       <c r="BG4">
+        <v>50619</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>9357631</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5">
+        <v>9357631</v>
+      </c>
+      <c r="L5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>9358034</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" t="s">
+        <v>74</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ5">
+        <v>9358034</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW5">
+        <v>35032001</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ5">
+        <v>4921569</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC5">
+        <v>35016742</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG5">
         <v>50619</v>
       </c>
     </row>
@@ -1429,6 +1608,11 @@
     <hyperlink ref="AY4" r:id="rId13" display="mailto:sudipt.d.sarkar@hsbc.co.in" xr:uid="{ACFEC149-83D1-C046-AA0F-CAA7BAC8E170}"/>
     <hyperlink ref="BB4" r:id="rId14" display="mailto:dominicparsons@hsbc.com" xr:uid="{EF2AA18E-49F7-954D-B1AE-871178400735}"/>
     <hyperlink ref="BE4" r:id="rId15" display="mailto:jimmy.k.c.mak@hsbc.com.hk" xr:uid="{591CDB83-736D-454C-947B-6B96745CB9E1}"/>
+    <hyperlink ref="G5" r:id="rId16" display="http://d3bxschxt4niqn.cloudfront.net/" xr:uid="{EB89FB51-6902-AA4D-980E-033B4CD33478}"/>
+    <hyperlink ref="AY5" r:id="rId17" display="mailto:sudipt.d.sarkar@hsbc.co.in" xr:uid="{1E7CDE72-F2F3-114D-8265-458F4EB2516F}"/>
+    <hyperlink ref="BB5" r:id="rId18" display="mailto:dominicparsons@hsbc.com" xr:uid="{C8D8676E-6C93-5C4E-A1ED-A1CA8C0DB3E6}"/>
+    <hyperlink ref="BE5" r:id="rId19" display="mailto:jimmy.k.c.mak@hsbc.com.hk" xr:uid="{2F7DD92B-D260-0040-B544-A0781327F427}"/>
+    <hyperlink ref="B5" r:id="rId20" display="www.google.com" xr:uid="{C6D39F82-7305-DE4F-82BE-C49CC35EE049}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>